<commit_message>
initialices renv and updated R version
</commit_message>
<xml_diff>
--- a/Belaege_Gewichtung.xlsx
+++ b/Belaege_Gewichtung.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="31" documentId="8_{72486D78-DEF3-48B5-ABEC-3983F2E8BA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03428A39-C63E-49F1-8C0E-8898EC50EE13}"/>
   <bookViews>
-    <workbookView xWindow="-34710" yWindow="2340" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-34710" yWindow="2340" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>